<commit_message>
update default data set
</commit_message>
<xml_diff>
--- a/test_data/swmm_data/gisswmm_inflows.xlsx
+++ b/test_data/swmm_data/gisswmm_inflows.xlsx
@@ -545,12 +545,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>dry_weather_hourly</t>
+          <t>"dry_weather_hourly"</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>dry_weather_monthly</t>
+          <t>"dry_weather_monthly"</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -558,11 +558,7 @@
           <t>""</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
-      </c>
+      <c r="G2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
add dividers to default data import
</commit_message>
<xml_diff>
--- a/test_data/swmm_data/gisswmm_inflows.xlsx
+++ b/test_data/swmm_data/gisswmm_inflows.xlsx
@@ -545,12 +545,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>dry_weather_hourly</t>
+          <t>"dry_weather_hourly"</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>dry_weather_monthly</t>
+          <t>"dry_weather_monthly"</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -558,11 +558,7 @@
           <t>""</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
-      </c>
+      <c r="G2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>